<commit_message>
save reach victim times
</commit_message>
<xml_diff>
--- a/Part_II/2_Data/Attack_Reaches_Victim_Times.xlsx
+++ b/Part_II/2_Data/Attack_Reaches_Victim_Times.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/39605/Documents/GitHub/2013_Fire_Attack/Part_II/2_Data/Laser/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/39605/Documents/GitHub/2013_Fire_Attack/Part_II/2_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8000" yWindow="3600" windowWidth="27220" windowHeight="16600" tabRatio="500"/>
+    <workbookView xWindow="1060" yWindow="460" windowWidth="29540" windowHeight="15440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="43">
   <si>
     <t>Experiment</t>
   </si>
@@ -123,12 +123,48 @@
   </si>
   <si>
     <t>Vic 1</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Std Dev</t>
+  </si>
+  <si>
+    <t>Victim 1 (sec)</t>
+  </si>
+  <si>
+    <t>Avg Interior</t>
+  </si>
+  <si>
+    <t>Avg Exterior</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min </t>
+  </si>
+  <si>
+    <t>Interior</t>
+  </si>
+  <si>
+    <t>Transitional</t>
+  </si>
+  <si>
+    <t>Difference</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -188,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -211,6 +247,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,45 +536,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:U38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="T32" sqref="T32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.5" customWidth="1"/>
-    <col min="14" max="14" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="0" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="12" customWidth="1"/>
+    <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="H1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="7"/>
-      <c r="N1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -563,14 +620,23 @@
       <c r="L2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="U2" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -609,14 +675,34 @@
       <c r="L3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="M3" s="12">
+        <v>19</v>
+      </c>
+      <c r="N3" s="12">
+        <v>32</v>
+      </c>
+      <c r="O3">
+        <f>N3+M3*60</f>
+        <v>1172</v>
+      </c>
+      <c r="P3">
+        <v>18</v>
+      </c>
+      <c r="Q3" s="8">
+        <v>33</v>
+      </c>
+      <c r="R3">
+        <f>Q3+P3*60</f>
+        <v>1113</v>
+      </c>
+      <c r="S3" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="P3" t="s">
+      <c r="U3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -655,16 +741,28 @@
       <c r="L4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="9">
-        <f>AVERAGE(K4:K13,K15:K18)</f>
-        <v>2.3974867724867698E-4</v>
-      </c>
-      <c r="P4" s="6">
-        <f>AVERAGE(H4:H13,H15:H20)</f>
-        <v>8.2175925925925906E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M4" s="12">
+        <v>1</v>
+      </c>
+      <c r="N4" s="12">
+        <v>19</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O26" si="2">N4+M4*60</f>
+        <v>79</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>22</v>
+      </c>
+      <c r="R4">
+        <f t="shared" ref="R4:R26" si="3">Q4+P4*60</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -703,8 +801,28 @@
       <c r="L5" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M5" s="12">
+        <v>0</v>
+      </c>
+      <c r="N5" s="12">
+        <v>54</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>12</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -743,14 +861,34 @@
       <c r="L6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="M6" s="12">
+        <v>0</v>
+      </c>
+      <c r="N6" s="12">
+        <v>54</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>20</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="S6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="P6" t="s">
+      <c r="U6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -789,16 +927,28 @@
       <c r="L7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N7" s="9">
-        <f>AVERAGE(K20,K22:K25)</f>
-        <v>4.5138888888888919E-4</v>
-      </c>
-      <c r="P7" s="6">
-        <f>AVERAGE(H22:H25,H20)</f>
-        <v>7.2453703703703742E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M7" s="12">
+        <v>0</v>
+      </c>
+      <c r="N7" s="12">
+        <v>59</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="2"/>
+        <v>59</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>21</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -837,8 +987,28 @@
       <c r="L8" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M8" s="12">
+        <v>1</v>
+      </c>
+      <c r="N8" s="12">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>23</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -877,8 +1047,28 @@
       <c r="L9" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M9" s="12">
+        <v>0</v>
+      </c>
+      <c r="N9" s="12">
+        <v>40</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>16</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -917,8 +1107,28 @@
       <c r="L10" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M10" s="12">
+        <v>0</v>
+      </c>
+      <c r="N10" s="12">
+        <v>58</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="8">
+        <v>28</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -957,8 +1167,28 @@
       <c r="L11" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M11" s="12">
+        <v>0</v>
+      </c>
+      <c r="N11" s="12">
+        <v>42</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>21</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -997,8 +1227,28 @@
       <c r="L12" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M12" s="12">
+        <v>0</v>
+      </c>
+      <c r="N12" s="12">
+        <v>55</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>20</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1037,8 +1287,28 @@
       <c r="L13" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M13" s="12">
+        <v>0</v>
+      </c>
+      <c r="N13" s="12">
+        <v>45</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>22</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1077,8 +1347,28 @@
       <c r="L14" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M14" s="12">
+        <v>8</v>
+      </c>
+      <c r="N14" s="12">
+        <v>14</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="2"/>
+        <v>494</v>
+      </c>
+      <c r="P14">
+        <v>7</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>39</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="3"/>
+        <v>459</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1117,8 +1407,28 @@
       <c r="L15" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M15" s="12">
+        <v>0</v>
+      </c>
+      <c r="N15" s="12">
+        <v>57</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>25</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1157,8 +1467,28 @@
       <c r="L16" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M16" s="12">
+        <v>0</v>
+      </c>
+      <c r="N16" s="12">
+        <v>55</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>21</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1197,8 +1527,28 @@
       <c r="L17" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M17" s="12">
+        <v>0</v>
+      </c>
+      <c r="N17" s="12">
+        <v>52</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="8">
+        <v>20</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1237,8 +1587,28 @@
       <c r="L18" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M18" s="12">
+        <v>0</v>
+      </c>
+      <c r="N18" s="12">
+        <v>45</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="8">
+        <v>19</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1277,8 +1647,28 @@
       <c r="L19" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M19" s="12">
+        <v>5</v>
+      </c>
+      <c r="N19" s="12">
+        <v>35</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="2"/>
+        <v>335</v>
+      </c>
+      <c r="P19">
+        <v>5</v>
+      </c>
+      <c r="Q19" s="8">
+        <v>12</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="3"/>
+        <v>312</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1317,8 +1707,28 @@
       <c r="L20" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M20" s="12">
+        <v>0</v>
+      </c>
+      <c r="N20" s="12">
+        <v>46</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="8">
+        <v>27</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1357,8 +1767,28 @@
       <c r="L21" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M21" s="12">
+        <v>4</v>
+      </c>
+      <c r="N21" s="12">
+        <v>10</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="2"/>
+        <v>250</v>
+      </c>
+      <c r="P21">
+        <v>3</v>
+      </c>
+      <c r="Q21" s="8">
+        <v>54</v>
+      </c>
+      <c r="R21">
+        <f t="shared" si="3"/>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1397,8 +1827,28 @@
       <c r="L22" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M22" s="12">
+        <v>1</v>
+      </c>
+      <c r="N22" s="12">
+        <v>2</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="2"/>
+        <v>62</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="8">
+        <v>49</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1437,8 +1887,28 @@
       <c r="L23" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M23" s="12">
+        <v>1</v>
+      </c>
+      <c r="N23" s="12">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="8">
+        <v>47</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1477,8 +1947,28 @@
       <c r="L24" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M24" s="12">
+        <v>1</v>
+      </c>
+      <c r="N24" s="12">
+        <v>17</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="2"/>
+        <v>77</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="8">
+        <v>36</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1517,8 +2007,28 @@
       <c r="L25" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M25" s="12">
+        <v>1</v>
+      </c>
+      <c r="N25" s="12">
+        <v>7</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="2"/>
+        <v>67</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="8">
+        <v>36</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1557,8 +2067,28 @@
       <c r="L26" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M26" s="12">
+        <v>1</v>
+      </c>
+      <c r="N26" s="12">
+        <v>42</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="2"/>
+        <v>102</v>
+      </c>
+      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="8">
+        <v>11</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="3"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -1575,8 +2105,10 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1608,10 +2140,304 @@
         <v>6</v>
       </c>
       <c r="K28" s="5">
-        <v>5.8796296296296296E-3</v>
+        <f>E28-G28</f>
+        <v>2.9861111111111108E-3</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="G29" t="s">
+        <v>32</v>
+      </c>
+      <c r="H29" s="6">
+        <f>AVERAGE(H4:H13,H15:H18,H20,H22:H26)</f>
+        <v>6.7708333333333325E-4</v>
+      </c>
+      <c r="K29" s="9">
+        <f>AVERAGE(K4:K13,K15:K18,K20,K22:K26)</f>
+        <v>3.2175925925925921E-4</v>
+      </c>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9">
+        <f t="shared" ref="M29:R29" si="4">AVERAGE(M4:M13,M15:M18,M20,M22:M26)</f>
+        <v>0.35</v>
+      </c>
+      <c r="N29" s="9">
+        <f t="shared" si="4"/>
+        <v>37.5</v>
+      </c>
+      <c r="O29" s="15">
+        <f t="shared" si="4"/>
+        <v>58.5</v>
+      </c>
+      <c r="P29" s="15">
+        <f t="shared" si="4"/>
+        <v>0.05</v>
+      </c>
+      <c r="Q29" s="15">
+        <f t="shared" si="4"/>
+        <v>24.8</v>
+      </c>
+      <c r="R29" s="15">
+        <f t="shared" si="4"/>
+        <v>27.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="G30" t="s">
+        <v>33</v>
+      </c>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11">
+        <f t="shared" ref="I30:R30" si="5">_xlfn.STDEV.P(M22:M26,M20,M15:M18,M4:M13)</f>
+        <v>0.47696960070847283</v>
+      </c>
+      <c r="N30" s="11">
+        <f t="shared" si="5"/>
+        <v>20.679700191250355</v>
+      </c>
+      <c r="O30" s="15">
+        <f>STDEV(O22:O26,O20,O15:O18,O4:O13)</f>
+        <v>14.496823608530322</v>
+      </c>
+      <c r="P30" s="15">
+        <f t="shared" si="5"/>
+        <v>0.21794494717703367</v>
+      </c>
+      <c r="Q30" s="15">
+        <f t="shared" si="5"/>
+        <v>9.8519033694002509</v>
+      </c>
+      <c r="R30" s="15">
+        <f>STDEV(R22:R26,R20,R15:R18,R4:R13)</f>
+        <v>13.964616941247959</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="G31" t="s">
+        <v>35</v>
+      </c>
+      <c r="H31" s="6">
+        <f>AVERAGE(H4:H13,H15:H18)</f>
+        <v>6.2417328042328019E-4</v>
+      </c>
+      <c r="K31" s="9">
+        <f>AVERAGE(K4:K13,K15:K18)</f>
+        <v>2.3974867724867698E-4</v>
+      </c>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9">
+        <f t="shared" ref="L31:R31" si="6">AVERAGE(M4:M13,M15:M18)</f>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="N31" s="9">
+        <f t="shared" si="6"/>
+        <v>45.357142857142854</v>
+      </c>
+      <c r="O31" s="15">
+        <f>AVERAGE(O4:O13,O15:O18)</f>
+        <v>53.928571428571431</v>
+      </c>
+      <c r="P31" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q31" s="15">
+        <f t="shared" si="6"/>
+        <v>20.714285714285715</v>
+      </c>
+      <c r="R31" s="15">
+        <f t="shared" si="6"/>
+        <v>20.714285714285715</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="G32" t="s">
+        <v>33</v>
+      </c>
+      <c r="O32" s="15">
+        <f>STDEV(O4:O13,O15:O18)</f>
+        <v>9.6831676771465833</v>
+      </c>
+      <c r="P32" s="15">
+        <f t="shared" ref="P32:R32" si="7">_xlfn.STDEV.P(P4:P13,P15:P18)</f>
+        <v>0</v>
+      </c>
+      <c r="Q32" s="15">
+        <f t="shared" si="7"/>
+        <v>3.6140316116210052</v>
+      </c>
+      <c r="R32" s="15">
+        <f>STDEV(R4:R13,R15:R18)</f>
+        <v>3.750457847507966</v>
+      </c>
+      <c r="S32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="7:20" x14ac:dyDescent="0.2">
+      <c r="G33" t="s">
+        <v>36</v>
+      </c>
+      <c r="H33" s="6">
+        <f>AVERAGE(H22:H26,H20)</f>
+        <v>8.0054012345679056E-4</v>
+      </c>
+      <c r="K33" s="9">
+        <f>AVERAGE(K20,K22:K26)</f>
+        <v>5.1311728395061758E-4</v>
+      </c>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9">
+        <f t="shared" ref="L33:R33" si="8">AVERAGE(M20,M22:M26)</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="N33" s="9">
+        <f t="shared" si="8"/>
+        <v>19.166666666666668</v>
+      </c>
+      <c r="O33" s="15">
+        <f>AVERAGE(O20,O22:O26)</f>
+        <v>69.166666666666671</v>
+      </c>
+      <c r="P33" s="15">
+        <f t="shared" si="8"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="Q33" s="15">
+        <f t="shared" si="8"/>
+        <v>34.333333333333336</v>
+      </c>
+      <c r="R33" s="15">
+        <f t="shared" si="8"/>
+        <v>44.333333333333336</v>
+      </c>
+      <c r="S33" s="15">
+        <f>O33-O31</f>
+        <v>15.238095238095241</v>
+      </c>
+      <c r="T33" s="15">
+        <f>R33-R31</f>
+        <v>23.61904761904762</v>
+      </c>
+    </row>
+    <row r="34" spans="7:20" x14ac:dyDescent="0.2">
+      <c r="G34" t="s">
+        <v>33</v>
+      </c>
+      <c r="O34">
+        <f>STDEV(O20,O22:O26)</f>
+        <v>18.967516091113946</v>
+      </c>
+      <c r="P34">
+        <f t="shared" ref="P34:R34" si="9">_xlfn.STDEV.P(P20,P22:P26)</f>
+        <v>0.37267799624996495</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="9"/>
+        <v>12.775845264491201</v>
+      </c>
+      <c r="R34">
+        <f>STDEV(R20,R22:R26)</f>
+        <v>15.357951252255843</v>
+      </c>
+    </row>
+    <row r="35" spans="7:20" x14ac:dyDescent="0.2">
+      <c r="K35" t="s">
+        <v>40</v>
+      </c>
+      <c r="L35" t="s">
+        <v>37</v>
+      </c>
+      <c r="O35">
+        <f>MIN(O4:O13,O15:O18)</f>
+        <v>40</v>
+      </c>
+      <c r="P35">
+        <f t="shared" ref="P35:R35" si="10">MIN(P4:P13,P15:P18)</f>
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="10"/>
+        <v>12</v>
+      </c>
+      <c r="R35">
+        <f>MIN(R4:R13,R15:R18)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="7:20" x14ac:dyDescent="0.2">
+      <c r="L36" t="s">
+        <v>38</v>
+      </c>
+      <c r="O36">
+        <f>MAX(O4:O13,O15:O18)</f>
+        <v>79</v>
+      </c>
+      <c r="P36">
+        <f t="shared" ref="P36:R36" si="11">MAX(P4:P13,P15:P18)</f>
+        <v>0</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="11"/>
+        <v>28</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="11"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="7:20" x14ac:dyDescent="0.2">
+      <c r="K37" t="s">
+        <v>41</v>
+      </c>
+      <c r="L37" t="s">
+        <v>39</v>
+      </c>
+      <c r="O37">
+        <f>MIN(O20,O22:O26)</f>
+        <v>46</v>
+      </c>
+      <c r="P37">
+        <f t="shared" ref="P37:R37" si="12">MIN(P20,P22:P26)</f>
+        <v>0</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="12"/>
+        <v>11</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="12"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="7:20" x14ac:dyDescent="0.2">
+      <c r="L38" t="s">
+        <v>38</v>
+      </c>
+      <c r="O38">
+        <f>MAX(O20,O22:O26)</f>
+        <v>102</v>
+      </c>
+      <c r="P38">
+        <f t="shared" ref="P38:R38" si="13">MAX(P20,P22:P26)</f>
+        <v>1</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="13"/>
+        <v>49</v>
+      </c>
+      <c r="R38">
+        <f t="shared" si="13"/>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>